<commit_message>
Update cad and list
</commit_message>
<xml_diff>
--- a/list_of_commodity/list_of_commodity.xlsx
+++ b/list_of_commodity/list_of_commodity.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Cost summary</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>M3*35</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>M3 螺帽</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -85,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>六角對邊: 5.5 厚度: 2.4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>白鐵螺絲 M3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -97,11 +89,102 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>不鏽鋼白鐵 m2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>M2*7 頭d : 3.2 thick : 1.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">AMP型 HID 接頭 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.5mm 端子 3P</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMP型 1.5mm端子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20 AWG線材</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sum :</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">紅 unit : 1M </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">黑 unit : 1M </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>祥昌電子</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>壓克力板加工</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>公</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>母</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>louishoma</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10mm 小開關 圓型開關</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>圓型開關</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M3*35 白鐵有頭內六角 unit : 10支</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>樂泰膠水 磁鐵 螺絲 螺帽 木工  塑膠螺絲(全館含稅附發票)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熱縮套管</t>
+  </si>
+  <si>
+    <t>4mm(黑) unit : 1m</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>阿宏</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>M2 螺帽</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>六角對邊: 4 厚度: 1.6 unit : 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">六角對邊: 5.5 厚度: 2.4 unit : 10 </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -109,7 +192,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +248,19 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -171,7 +270,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -194,25 +293,61 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="貨幣" xfId="2" builtinId="4"/>
     <cellStyle name="超連結" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
@@ -506,10 +641,10 @@
     <col min="5" max="5" width="14.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19.125" customWidth="1"/>
     <col min="7" max="7" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.125" customWidth="1"/>
+    <col min="9" max="9" width="96.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" ht="30.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -519,9 +654,9 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-    </row>
-    <row r="2" spans="1:8" ht="31.2" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I1" s="2"/>
+    </row>
+    <row r="2" spans="1:9" ht="31.2" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -544,148 +679,412 @@
         <v>5</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
         <v>1</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="10">
+        <v>318</v>
+      </c>
+      <c r="E3" s="5">
+        <v>1</v>
+      </c>
+      <c r="F3" s="10">
+        <v>60</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G4" si="0">D3*E3+F3</f>
+        <v>378</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D4" s="10">
         <v>2</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E4" s="5">
         <v>20</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6">
-        <f>D3*E3+F3</f>
+      <c r="F4" s="10">
+        <v>60</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>3</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="10">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10">
+        <v>60</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" ref="G5:G8" si="1">D5*E5+F5</f>
+        <v>100</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>3</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="D6" s="10">
+        <v>10</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10">
+        <f t="shared" ref="G6" si="2">D6*E6+F6</f>
+        <v>20</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="10">
+        <v>10</v>
+      </c>
+      <c r="E7" s="5">
+        <v>2</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="10">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5">
+        <v>2</v>
+      </c>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>6</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="10">
+        <v>25</v>
+      </c>
+      <c r="E9" s="5">
+        <v>6</v>
+      </c>
+      <c r="F9" s="10">
+        <v>60</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" ref="G9:G13" si="3">D9*E9+F9</f>
+        <v>210</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>7</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="5">
+        <v>15</v>
+      </c>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>15</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10">
+        <f t="shared" ref="G11" si="4">D11*E11+F11</f>
+        <v>45</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>9</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="10">
+        <v>15</v>
+      </c>
+      <c r="E12" s="5">
+        <v>3</v>
+      </c>
+      <c r="F12" s="10">
+        <v>60</v>
+      </c>
+      <c r="G12" s="10">
+        <f>D12*E12+F12</f>
+        <v>105</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2</v>
-      </c>
-      <c r="E4" s="6">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6">
-        <f t="shared" ref="G4:G8" si="0">D4*E4</f>
-        <v>40</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="B13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="10">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
-      </c>
-      <c r="E5" s="6">
-        <v>20</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
-        <v>4</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="H13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>11</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="10">
+        <v>7</v>
+      </c>
+      <c r="E14" s="5">
         <v>3</v>
       </c>
-      <c r="E6" s="6">
-        <v>20</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
-        <v>5</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="5">
-        <v>6</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H8" s="6"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10">
+        <f t="shared" ref="G14" si="5">D14*E14+F14</f>
+        <v>21</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>12</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="10">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10">
+        <f t="shared" ref="G15" si="6">D15*E15+F15</f>
+        <v>36</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="13"/>
+      <c r="F16" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="11">
+        <f>SUM(G3:G14)</f>
+        <v>1112</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="H3" r:id="rId1"/>
-    <hyperlink ref="H5" r:id="rId2" display="m2不鏽鋼螺帽"/>
-    <hyperlink ref="H6" r:id="rId3"/>
-    <hyperlink ref="H4" r:id="rId4"/>
+    <hyperlink ref="I7" r:id="rId1" display="m2不鏽鋼螺帽"/>
+    <hyperlink ref="I8" r:id="rId2"/>
+    <hyperlink ref="I13" r:id="rId3"/>
+    <hyperlink ref="I14" r:id="rId4"/>
+    <hyperlink ref="I4" r:id="rId5"/>
+    <hyperlink ref="I9" r:id="rId6"/>
+    <hyperlink ref="I10" r:id="rId7"/>
+    <hyperlink ref="I11" r:id="rId8"/>
+    <hyperlink ref="I12" r:id="rId9"/>
+    <hyperlink ref="I5" r:id="rId10"/>
+    <hyperlink ref="I15" r:id="rId11"/>
+    <hyperlink ref="I3" r:id="rId12"/>
+    <hyperlink ref="I6" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>